<commit_message>
corrigé erreur de typo
</commit_message>
<xml_diff>
--- a/Retroplanning.xlsx
+++ b/Retroplanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anas1\Documents\clone-ps6\2019-2020-ps6-rendu-rip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E85F1E-5999-43EA-9A6B-1BF84F04EBB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA4E270-F6BF-42E4-AE77-A52039F56E71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">Affichage réponses juste </t>
   </si>
   <si>
-    <t xml:space="preserve">Au fure et à meusure </t>
+    <t xml:space="preserve">Au fur et à mesure </t>
   </si>
 </sst>
 </file>
@@ -203,10 +203,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -492,7 +492,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -830,29 +830,29 @@
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">

</xml_diff>